<commit_message>
Changed Jim Molan to an active denier
</commit_message>
<xml_diff>
--- a/data/Senate.xlsx
+++ b/data/Senate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python\Govt Climate Denialists\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4CE8DC1-C156-486F-B4DD-2C159221E18F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D29CD69-56F6-4AE5-964E-AF350131906E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6225" yWindow="2025" windowWidth="28800" windowHeight="15435" xr2:uid="{E1023773-23E4-46BF-9D85-6FF2DA1565CC}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{E1023773-23E4-46BF-9D85-6FF2DA1565CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="140">
   <si>
     <t>Hon. Eric Abetz</t>
   </si>
@@ -531,6 +531,9 @@
   </si>
   <si>
     <t>Long history of outspoken climate denial</t>
+  </si>
+  <si>
+    <t>“As to whether it is human-induced climate change … 'I'm not relying on evidence' for climate change" - Q&amp;A 3/2/20</t>
   </si>
 </sst>
 </file>
@@ -959,8 +962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAC1B42C-9515-4F57-AADB-1E0B8EA7A71B}">
   <dimension ref="A1:H77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F89" sqref="F89"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="N50" sqref="N50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2092,10 +2095,13 @@
         <v>83</v>
       </c>
       <c r="F48" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G48" t="s">
         <v>129</v>
+      </c>
+      <c r="H48" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>